<commit_message>
Second Stage registration added
</commit_message>
<xml_diff>
--- a/Documentation/literature research/Gant chart.xlsx
+++ b/Documentation/literature research/Gant chart.xlsx
@@ -141,11 +141,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="dd\-mmm"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="dd\-mmm"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -177,6 +177,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -184,6 +192,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -191,8 +215,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -201,45 +248,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -253,6 +261,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -276,48 +292,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -384,157 +384,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -545,6 +545,39 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -578,39 +611,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -629,8 +629,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -648,7 +648,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -666,119 +666,119 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -915,10 +915,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="D4D4D4"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="202020"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>

</xml_diff>

<commit_message>
Members can be added to Rooms
</commit_message>
<xml_diff>
--- a/Documentation/literature research/Gant chart.xlsx
+++ b/Documentation/literature research/Gant chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12585"/>
+    <workbookView windowWidth="15360" windowHeight="15585"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </t>
   </si>
   <si>
-    <t>Allow users to draw on the same canvas</t>
+    <t xml:space="preserve">Allow users to draw on the same canvas </t>
   </si>
   <si>
     <t>Create chat box for a room</t>
@@ -99,7 +99,7 @@
     <t>Display rooms joined for each user</t>
   </si>
   <si>
-    <t>Auto Saving canvas</t>
+    <t xml:space="preserve">Auto Saving canvas and create 3 art tools </t>
   </si>
   <si>
     <t>Style frontend</t>
@@ -141,11 +141,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="dd\-mmm"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -179,24 +179,100 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -209,115 +285,39 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -366,169 +366,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -557,11 +557,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -581,32 +587,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -635,6 +620,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -666,124 +666,124 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="8" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="31" applyFont="1"/>
@@ -812,25 +812,30 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="176" fontId="3" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="176" fontId="3" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -839,12 +844,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1171,7 +1170,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1401,16 +1400,16 @@
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="7"/>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="9">
         <v>44203</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="9">
         <v>44203</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1418,16 +1417,16 @@
     </row>
     <row r="14" ht="30" spans="1:6">
       <c r="A14" s="7"/>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="9">
         <v>44204</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="9">
         <v>44206</v>
       </c>
-      <c r="E14" s="19">
+      <c r="E14" s="10">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
@@ -1435,16 +1434,16 @@
     </row>
     <row r="15" ht="13.5" customHeight="1" spans="1:6">
       <c r="A15" s="7"/>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="9">
         <v>44208</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="9">
         <v>44208</v>
       </c>
-      <c r="E15" s="19">
+      <c r="E15" s="10">
         <f t="shared" ref="E15:E30" si="1">D15-C15</f>
         <v>0</v>
       </c>
@@ -1454,16 +1453,16 @@
       <c r="A16" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="16">
         <v>44148</v>
       </c>
-      <c r="D16" s="22">
+      <c r="D16" s="16">
         <v>44149</v>
       </c>
-      <c r="E16" s="23">
+      <c r="E16" s="17">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1471,16 +1470,16 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="7"/>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="22">
+      <c r="C17" s="19">
         <v>44211</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="19">
         <v>44216</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="20">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -1488,16 +1487,16 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="7"/>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="9">
         <v>44217</v>
       </c>
-      <c r="D18" s="22">
+      <c r="D18" s="9">
         <v>44219</v>
       </c>
-      <c r="E18" s="23">
+      <c r="E18" s="10">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1505,16 +1504,16 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="7"/>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="22">
+      <c r="C19" s="19">
         <v>44220</v>
       </c>
-      <c r="D19" s="22">
+      <c r="D19" s="19">
         <v>44221</v>
       </c>
-      <c r="E19" s="23">
+      <c r="E19" s="20">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1522,16 +1521,16 @@
     </row>
     <row r="20" ht="30.75" customHeight="1" spans="1:6">
       <c r="A20" s="7"/>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="19">
         <v>44222</v>
       </c>
-      <c r="D20" s="22">
+      <c r="D20" s="19">
         <v>44227</v>
       </c>
-      <c r="E20" s="23">
+      <c r="E20" s="20">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
@@ -1539,16 +1538,16 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="7"/>
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="19">
         <v>44228</v>
       </c>
-      <c r="D21" s="22">
+      <c r="D21" s="19">
         <v>44229</v>
       </c>
-      <c r="E21" s="23">
+      <c r="E21" s="20">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1556,16 +1555,16 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="7"/>
-      <c r="B22" s="24" t="s">
+      <c r="B22" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="22">
+      <c r="C22" s="19">
         <v>44230</v>
       </c>
-      <c r="D22" s="22">
+      <c r="D22" s="19">
         <v>44231</v>
       </c>
-      <c r="E22" s="23">
+      <c r="E22" s="20">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1575,16 +1574,16 @@
       <c r="A23" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="22">
+      <c r="C23" s="23">
         <v>44234</v>
       </c>
-      <c r="D23" s="22">
+      <c r="D23" s="23">
         <v>44237</v>
       </c>
-      <c r="E23" s="23">
+      <c r="E23" s="24">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -1592,16 +1591,16 @@
     </row>
     <row r="24" ht="30" spans="1:6">
       <c r="A24" s="7"/>
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="22">
+      <c r="C24" s="23">
         <v>44238</v>
       </c>
-      <c r="D24" s="22">
+      <c r="D24" s="23">
         <v>44241</v>
       </c>
-      <c r="E24" s="23">
+      <c r="E24" s="24">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -1609,16 +1608,16 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="7"/>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="22">
+      <c r="C25" s="23">
         <v>44242</v>
       </c>
-      <c r="D25" s="22">
+      <c r="D25" s="23">
         <v>44244</v>
       </c>
-      <c r="E25" s="23">
+      <c r="E25" s="24">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1626,16 +1625,16 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="7"/>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="22">
+      <c r="C26" s="23">
         <v>44245</v>
       </c>
-      <c r="D26" s="22">
+      <c r="D26" s="23">
         <v>44247</v>
       </c>
-      <c r="E26" s="23">
+      <c r="E26" s="24">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1645,16 +1644,16 @@
       <c r="A27" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="22">
+      <c r="C27" s="23">
         <v>44248</v>
       </c>
-      <c r="D27" s="22">
+      <c r="D27" s="23">
         <v>44250</v>
       </c>
-      <c r="E27" s="23">
+      <c r="E27" s="24">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1662,16 +1661,16 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="7"/>
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="22">
+      <c r="C28" s="23">
         <v>44251</v>
       </c>
-      <c r="D28" s="22">
+      <c r="D28" s="23">
         <v>44253</v>
       </c>
-      <c r="E28" s="23">
+      <c r="E28" s="24">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1679,16 +1678,16 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="7"/>
-      <c r="B29" s="24" t="s">
+      <c r="B29" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="22">
+      <c r="C29" s="23">
         <v>44253</v>
       </c>
-      <c r="D29" s="22">
+      <c r="D29" s="23">
         <v>44255</v>
       </c>
-      <c r="E29" s="23">
+      <c r="E29" s="24">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1696,17 +1695,17 @@
     </row>
     <row r="30" spans="4:5">
       <c r="D30" s="11"/>
-      <c r="E30" s="28"/>
+      <c r="E30" s="27"/>
     </row>
     <row r="31" spans="4:5">
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
+      <c r="D31" s="27"/>
+      <c r="E31" s="27"/>
     </row>
     <row r="32" spans="5:5">
-      <c r="E32" s="28"/>
+      <c r="E32" s="27"/>
     </row>
     <row r="33" spans="5:5">
-      <c r="E33" s="28"/>
+      <c r="E33" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Join/create and leave rooms
</commit_message>
<xml_diff>
--- a/Documentation/literature research/Gant chart.xlsx
+++ b/Documentation/literature research/Gant chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="15360" windowHeight="15585"/>
+    <workbookView windowWidth="28800" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -141,13 +141,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="dd\-mmm"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="dd\-mmm"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +177,65 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -185,61 +244,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -285,14 +292,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -366,7 +373,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.8"/>
+        <fgColor theme="9" tint="0.6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -384,19 +391,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -408,25 +499,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -438,103 +535,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -545,15 +552,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -590,6 +588,24 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4"/>
       </bottom>
@@ -607,15 +623,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -648,7 +655,7 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -666,124 +673,124 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="8" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="31" applyFont="1"/>
@@ -815,14 +822,24 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="176" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="176" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="176" fontId="3" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -830,9 +847,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1169,8 +1183,8 @@
   <sheetPr/>
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E17" sqref="B17:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1504,16 +1518,16 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="7"/>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="19">
+      <c r="C19" s="9">
         <v>44220</v>
       </c>
-      <c r="D19" s="19">
+      <c r="D19" s="9">
         <v>44221</v>
       </c>
-      <c r="E19" s="20">
+      <c r="E19" s="10">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1538,16 +1552,16 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="7"/>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="19">
+      <c r="C21" s="9">
         <v>44228</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="9">
         <v>44229</v>
       </c>
-      <c r="E21" s="20">
+      <c r="E21" s="10">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1555,16 +1569,16 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="7"/>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="19">
+      <c r="C22" s="23">
         <v>44230</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="23">
         <v>44231</v>
       </c>
-      <c r="E22" s="20">
+      <c r="E22" s="24">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1574,16 +1588,16 @@
       <c r="A23" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="23">
+      <c r="C23" s="26">
         <v>44234</v>
       </c>
-      <c r="D23" s="23">
+      <c r="D23" s="26">
         <v>44237</v>
       </c>
-      <c r="E23" s="24">
+      <c r="E23" s="27">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -1591,16 +1605,16 @@
     </row>
     <row r="24" ht="30" spans="1:6">
       <c r="A24" s="7"/>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="23">
+      <c r="C24" s="26">
         <v>44238</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24" s="26">
         <v>44241</v>
       </c>
-      <c r="E24" s="24">
+      <c r="E24" s="27">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
@@ -1608,16 +1622,16 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="7"/>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="23">
+      <c r="C25" s="26">
         <v>44242</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="26">
         <v>44244</v>
       </c>
-      <c r="E25" s="24">
+      <c r="E25" s="27">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1625,16 +1639,16 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="7"/>
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="23">
+      <c r="C26" s="26">
         <v>44245</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="26">
         <v>44247</v>
       </c>
-      <c r="E26" s="24">
+      <c r="E26" s="27">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1644,16 +1658,16 @@
       <c r="A27" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="23">
+      <c r="C27" s="26">
         <v>44248</v>
       </c>
-      <c r="D27" s="23">
+      <c r="D27" s="26">
         <v>44250</v>
       </c>
-      <c r="E27" s="24">
+      <c r="E27" s="27">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1661,16 +1675,16 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="7"/>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="23">
+      <c r="C28" s="26">
         <v>44251</v>
       </c>
-      <c r="D28" s="23">
+      <c r="D28" s="26">
         <v>44253</v>
       </c>
-      <c r="E28" s="24">
+      <c r="E28" s="27">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1678,16 +1692,16 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="7"/>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="23">
+      <c r="C29" s="26">
         <v>44253</v>
       </c>
-      <c r="D29" s="23">
+      <c r="D29" s="26">
         <v>44255</v>
       </c>
-      <c r="E29" s="24">
+      <c r="E29" s="27">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1695,17 +1709,17 @@
     </row>
     <row r="30" spans="4:5">
       <c r="D30" s="11"/>
-      <c r="E30" s="27"/>
+      <c r="E30" s="30"/>
     </row>
     <row r="31" spans="4:5">
-      <c r="D31" s="27"/>
-      <c r="E31" s="27"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
     </row>
     <row r="32" spans="5:5">
-      <c r="E32" s="27"/>
+      <c r="E32" s="30"/>
     </row>
     <row r="33" spans="5:5">
-      <c r="E33" s="27"/>
+      <c r="E33" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Live drawing and layering added
</commit_message>
<xml_diff>
--- a/Documentation/literature research/Gant chart.xlsx
+++ b/Documentation/literature research/Gant chart.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Phase</t>
   </si>
@@ -99,16 +99,19 @@
     <t>Display rooms joined for each user</t>
   </si>
   <si>
-    <t xml:space="preserve">Auto Saving canvas and create 3 art tools </t>
+    <t xml:space="preserve">Create 3 art tools: Brush, eraser , color picker </t>
+  </si>
+  <si>
+    <t>Auto Saving canvas</t>
   </si>
   <si>
     <t>Style frontend</t>
   </si>
   <si>
+    <t>Iteration 4</t>
+  </si>
+  <si>
     <t>Monitor user's mood for front end</t>
-  </si>
-  <si>
-    <t>Iteration 4</t>
   </si>
   <si>
     <t>Require user to make a request before 
@@ -121,10 +124,10 @@
     <t>Allow user to accept/decline request</t>
   </si>
   <si>
+    <t>Iteration 5</t>
+  </si>
+  <si>
     <t>Add livestream preview in room page</t>
-  </si>
-  <si>
-    <t>Iteration 5</t>
   </si>
   <si>
     <t>Add voice chat to room</t>
@@ -142,10 +145,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="dd\-mmm"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="dd\-mmm"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -184,17 +187,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -208,45 +210,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -260,8 +232,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -275,14 +286,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -292,39 +295,39 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -391,37 +394,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -433,115 +544,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -556,16 +559,36 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -588,41 +611,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -644,18 +649,16 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -673,124 +676,124 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="8" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="31" applyFont="1"/>
@@ -831,15 +834,14 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="176" fontId="3" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1181,10 +1183,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E17" sqref="B17:E17"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1458,7 +1460,7 @@
         <v>44208</v>
       </c>
       <c r="E15" s="10">
-        <f t="shared" ref="E15:E30" si="1">D15-C15</f>
+        <f>D15-C15</f>
         <v>0</v>
       </c>
       <c r="F15" s="11"/>
@@ -1477,24 +1479,24 @@
         <v>44149</v>
       </c>
       <c r="E16" s="17">
-        <f t="shared" si="1"/>
+        <f>D16-C16</f>
         <v>1</v>
       </c>
       <c r="F16" s="11"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="7"/>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="19">
+      <c r="C17" s="9">
         <v>44211</v>
       </c>
-      <c r="D17" s="19">
+      <c r="D17" s="9">
         <v>44216</v>
       </c>
-      <c r="E17" s="20">
-        <f t="shared" si="1"/>
+      <c r="E17" s="10">
+        <f>D17-C17</f>
         <v>5</v>
       </c>
       <c r="F17" s="11"/>
@@ -1511,7 +1513,7 @@
         <v>44219</v>
       </c>
       <c r="E18" s="10">
-        <f t="shared" si="1"/>
+        <f>D18-C18</f>
         <v>2</v>
       </c>
       <c r="F18" s="11"/>
@@ -1528,127 +1530,122 @@
         <v>44221</v>
       </c>
       <c r="E19" s="10">
+        <f>D19-C19</f>
+        <v>1</v>
+      </c>
+      <c r="F19" s="11"/>
+    </row>
+    <row r="20" ht="30.75" customHeight="1" spans="1:6">
+      <c r="A20" s="7"/>
+      <c r="B20" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="19">
+        <v>44222</v>
+      </c>
+      <c r="D20" s="19">
+        <v>44227</v>
+      </c>
+      <c r="E20" s="20">
+        <f>D20-C20</f>
+        <v>5</v>
+      </c>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="7"/>
+      <c r="B21" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="20">
+        <v>5</v>
+      </c>
+      <c r="F21" s="11"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="7"/>
+      <c r="B22" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="9">
+        <v>44228</v>
+      </c>
+      <c r="D22" s="9">
+        <v>44229</v>
+      </c>
+      <c r="E22" s="10">
+        <f t="shared" ref="E22:E31" si="1">D22-C22</f>
+        <v>1</v>
+      </c>
+      <c r="F22" s="11"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="22">
+        <v>44230</v>
+      </c>
+      <c r="D23" s="22">
+        <v>44231</v>
+      </c>
+      <c r="E23" s="23">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="F19" s="11"/>
-    </row>
-    <row r="20" ht="30.75" customHeight="1" spans="1:6">
-      <c r="A20" s="7"/>
-      <c r="B20" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="19">
-        <v>44222</v>
-      </c>
-      <c r="D20" s="19">
-        <v>44227</v>
-      </c>
-      <c r="E20" s="20">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="F20" s="11"/>
-    </row>
-    <row r="21" spans="1:6">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="9">
-        <v>44228</v>
-      </c>
-      <c r="D21" s="9">
-        <v>44229</v>
-      </c>
-      <c r="E21" s="10">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F21" s="11"/>
-    </row>
-    <row r="22" spans="1:6">
-      <c r="A22" s="7"/>
-      <c r="B22" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="23">
-        <v>44230</v>
-      </c>
-      <c r="D22" s="23">
-        <v>44231</v>
-      </c>
-      <c r="E22" s="24">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F22" s="11"/>
-    </row>
-    <row r="23" ht="30" spans="1:6">
-      <c r="A23" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" s="26">
+      <c r="F23" s="11"/>
+    </row>
+    <row r="24" ht="30" spans="1:6">
+      <c r="A24" s="7"/>
+      <c r="B24" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" s="25">
         <v>44234</v>
       </c>
-      <c r="D23" s="26">
+      <c r="D24" s="25">
         <v>44237</v>
       </c>
-      <c r="E23" s="27">
+      <c r="E24" s="26">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F23" s="11"/>
-    </row>
-    <row r="24" ht="30" spans="1:6">
-      <c r="A24" s="7"/>
-      <c r="B24" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="26">
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" ht="30" spans="1:6">
+      <c r="A25" s="7"/>
+      <c r="B25" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="25">
         <v>44238</v>
       </c>
-      <c r="D24" s="26">
+      <c r="D25" s="25">
         <v>44241</v>
       </c>
-      <c r="E24" s="27">
+      <c r="E25" s="26">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F24" s="11"/>
-    </row>
-    <row r="25" spans="1:6">
-      <c r="A25" s="7"/>
-      <c r="B25" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="26">
-        <v>44242</v>
-      </c>
-      <c r="D25" s="26">
-        <v>44244</v>
-      </c>
-      <c r="E25" s="27">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
       <c r="F25" s="11"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="7"/>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="26">
-        <v>44245</v>
-      </c>
-      <c r="D26" s="26">
-        <v>44247</v>
-      </c>
-      <c r="E26" s="27">
+      <c r="C26" s="25">
+        <v>44242</v>
+      </c>
+      <c r="D26" s="25">
+        <v>44244</v>
+      </c>
+      <c r="E26" s="26">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1661,13 +1658,13 @@
       <c r="B27" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="26">
-        <v>44248</v>
-      </c>
-      <c r="D27" s="26">
-        <v>44250</v>
-      </c>
-      <c r="E27" s="27">
+      <c r="C27" s="25">
+        <v>44245</v>
+      </c>
+      <c r="D27" s="25">
+        <v>44247</v>
+      </c>
+      <c r="E27" s="26">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1675,16 +1672,16 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="7"/>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="26">
-        <v>44251</v>
-      </c>
-      <c r="D28" s="26">
-        <v>44253</v>
-      </c>
-      <c r="E28" s="27">
+      <c r="C28" s="25">
+        <v>44248</v>
+      </c>
+      <c r="D28" s="25">
+        <v>44250</v>
+      </c>
+      <c r="E28" s="26">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -1692,43 +1689,60 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="7"/>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="26">
+      <c r="C29" s="25">
+        <v>44251</v>
+      </c>
+      <c r="D29" s="25">
         <v>44253</v>
       </c>
-      <c r="D29" s="26">
-        <v>44255</v>
-      </c>
-      <c r="E29" s="27">
+      <c r="E29" s="26">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="F29" s="11"/>
     </row>
-    <row r="30" spans="4:5">
-      <c r="D30" s="11"/>
-      <c r="E30" s="30"/>
+    <row r="30" spans="2:5">
+      <c r="B30" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="25">
+        <v>44253</v>
+      </c>
+      <c r="D30" s="25">
+        <v>44255</v>
+      </c>
+      <c r="E30" s="26">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="31" spans="4:5">
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
-    </row>
-    <row r="32" spans="5:5">
-      <c r="E32" s="30"/>
+      <c r="D31" s="11"/>
+      <c r="E31" s="29"/>
+    </row>
+    <row r="32" spans="4:5">
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
     </row>
     <row r="33" spans="5:5">
-      <c r="E33" s="30"/>
+      <c r="E33" s="29"/>
+    </row>
+    <row r="34" spans="5:5">
+      <c r="E34" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="8">
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A10"/>
     <mergeCell ref="A11:A15"/>
     <mergeCell ref="A16:A22"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="A27:A29"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait"/>

</xml_diff>